<commit_message>
format date in excel
</commit_message>
<xml_diff>
--- a/src/Samples/testoutput.xlsx
+++ b/src/Samples/testoutput.xlsx
@@ -5,7 +5,7 @@
     <workbookView/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr fullCalcOnLoad="1"/>
 </workbook>
@@ -312,7 +312,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="dd/MM/yyyy"/>
+  </numFmts>
   <fonts count="1">
     <font>
       <sz val="11"/>
@@ -336,14 +338,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0"/>
+    <xf numFmtId="164" fontId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" xfId="0"/>
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0"/>
+    <xf numFmtId="164" applyNumberFormat="1" fontId="0" applyFont="1" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Date" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
 </styleSheet>
@@ -354,7 +359,7 @@
   <autoFilter ref="A1:B97"/>
   <tableColumns count="2">
     <tableColumn id="1" name="TheName"/>
-    <tableColumn id="2" name="Modified"/>
+    <tableColumn id="2" name="Modified" dataCellStyle="Date"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -369,7 +374,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="58.4935989379883" customWidth="1"/>
-    <col min="2" max="2" width="12.8945598602295" customWidth="1"/>
+    <col min="2" max="2" width="11.8295488357544" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -384,7 +389,7 @@
       <c r="A2" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="0">
+      <c r="B2" s="1">
         <v>43350.0950182755</v>
       </c>
     </row>
@@ -392,7 +397,7 @@
       <c r="A3" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="0">
+      <c r="B3" s="1">
         <v>43350.0950182755</v>
       </c>
     </row>
@@ -400,7 +405,7 @@
       <c r="A4" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="0">
+      <c r="B4" s="1">
         <v>43350.0950182755</v>
       </c>
     </row>
@@ -408,7 +413,7 @@
       <c r="A5" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="0">
+      <c r="B5" s="1">
         <v>43350.0950182755</v>
       </c>
     </row>
@@ -416,7 +421,7 @@
       <c r="A6" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="0">
+      <c r="B6" s="1">
         <v>43350.0950182755</v>
       </c>
     </row>
@@ -424,7 +429,7 @@
       <c r="A7" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="0">
+      <c r="B7" s="1">
         <v>43350.0950182755</v>
       </c>
     </row>
@@ -432,7 +437,7 @@
       <c r="A8" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="0">
+      <c r="B8" s="1">
         <v>43350.0950182755</v>
       </c>
     </row>
@@ -440,7 +445,7 @@
       <c r="A9" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="0">
+      <c r="B9" s="1">
         <v>43350.0950182755</v>
       </c>
     </row>
@@ -448,7 +453,7 @@
       <c r="A10" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="0">
+      <c r="B10" s="1">
         <v>43350.0950182755</v>
       </c>
     </row>
@@ -456,7 +461,7 @@
       <c r="A11" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="0">
+      <c r="B11" s="1">
         <v>43350.0950182755</v>
       </c>
     </row>
@@ -464,7 +469,7 @@
       <c r="A12" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="0">
+      <c r="B12" s="1">
         <v>43350.0950182755</v>
       </c>
     </row>
@@ -472,7 +477,7 @@
       <c r="A13" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="0">
+      <c r="B13" s="1">
         <v>43350.0950182755</v>
       </c>
     </row>
@@ -480,7 +485,7 @@
       <c r="A14" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="0">
+      <c r="B14" s="1">
         <v>43350.0950182755</v>
       </c>
     </row>
@@ -488,7 +493,7 @@
       <c r="A15" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="0">
+      <c r="B15" s="1">
         <v>43350.0950182755</v>
       </c>
     </row>
@@ -496,7 +501,7 @@
       <c r="A16" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="0">
+      <c r="B16" s="1">
         <v>43350.0950182755</v>
       </c>
     </row>
@@ -504,7 +509,7 @@
       <c r="A17" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="0">
+      <c r="B17" s="1">
         <v>43350.0950182755</v>
       </c>
     </row>
@@ -512,7 +517,7 @@
       <c r="A18" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="0">
+      <c r="B18" s="1">
         <v>43350.0950182755</v>
       </c>
     </row>
@@ -520,7 +525,7 @@
       <c r="A19" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="0">
+      <c r="B19" s="1">
         <v>43350.0950182755</v>
       </c>
     </row>
@@ -528,7 +533,7 @@
       <c r="A20" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="0">
+      <c r="B20" s="1">
         <v>43350.0950182755</v>
       </c>
     </row>
@@ -536,7 +541,7 @@
       <c r="A21" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="B21" s="0">
+      <c r="B21" s="1">
         <v>43350.0950182755</v>
       </c>
     </row>
@@ -544,7 +549,7 @@
       <c r="A22" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="B22" s="0">
+      <c r="B22" s="1">
         <v>43350.0950182755</v>
       </c>
     </row>
@@ -552,7 +557,7 @@
       <c r="A23" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="B23" s="0">
+      <c r="B23" s="1">
         <v>43350.0950182755</v>
       </c>
     </row>
@@ -560,7 +565,7 @@
       <c r="A24" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="B24" s="0">
+      <c r="B24" s="1">
         <v>43350.0950182755</v>
       </c>
     </row>
@@ -568,7 +573,7 @@
       <c r="A25" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="B25" s="0">
+      <c r="B25" s="1">
         <v>43350.0950182755</v>
       </c>
     </row>
@@ -576,7 +581,7 @@
       <c r="A26" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="B26" s="0">
+      <c r="B26" s="1">
         <v>43350.0950182755</v>
       </c>
     </row>
@@ -584,7 +589,7 @@
       <c r="A27" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="B27" s="0">
+      <c r="B27" s="1">
         <v>43350.0950182755</v>
       </c>
     </row>
@@ -592,7 +597,7 @@
       <c r="A28" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="B28" s="0">
+      <c r="B28" s="1">
         <v>43350.0950182755</v>
       </c>
     </row>
@@ -600,7 +605,7 @@
       <c r="A29" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="B29" s="0">
+      <c r="B29" s="1">
         <v>43350.0950182755</v>
       </c>
     </row>
@@ -608,7 +613,7 @@
       <c r="A30" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="B30" s="0">
+      <c r="B30" s="1">
         <v>43350.0950182755</v>
       </c>
     </row>
@@ -616,7 +621,7 @@
       <c r="A31" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="B31" s="0">
+      <c r="B31" s="1">
         <v>43350.0950182755</v>
       </c>
     </row>
@@ -624,7 +629,7 @@
       <c r="A32" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="B32" s="0">
+      <c r="B32" s="1">
         <v>43350.0950182755</v>
       </c>
     </row>
@@ -632,7 +637,7 @@
       <c r="A33" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="B33" s="0">
+      <c r="B33" s="1">
         <v>43350.0950182755</v>
       </c>
     </row>
@@ -640,7 +645,7 @@
       <c r="A34" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="B34" s="0">
+      <c r="B34" s="1">
         <v>43350.0920083796</v>
       </c>
     </row>
@@ -648,7 +653,7 @@
       <c r="A35" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="B35" s="0">
+      <c r="B35" s="1">
         <v>43350.0920083796</v>
       </c>
     </row>
@@ -656,7 +661,7 @@
       <c r="A36" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="B36" s="0">
+      <c r="B36" s="1">
         <v>43350.0920083796</v>
       </c>
     </row>
@@ -664,7 +669,7 @@
       <c r="A37" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="B37" s="0">
+      <c r="B37" s="1">
         <v>43350.0920083796</v>
       </c>
     </row>
@@ -672,7 +677,7 @@
       <c r="A38" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="B38" s="0">
+      <c r="B38" s="1">
         <v>43350.0920083796</v>
       </c>
     </row>
@@ -680,7 +685,7 @@
       <c r="A39" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="B39" s="0">
+      <c r="B39" s="1">
         <v>43350.0920083796</v>
       </c>
     </row>
@@ -688,7 +693,7 @@
       <c r="A40" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="B40" s="0">
+      <c r="B40" s="1">
         <v>43350.0920083796</v>
       </c>
     </row>
@@ -696,7 +701,7 @@
       <c r="A41" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="B41" s="0">
+      <c r="B41" s="1">
         <v>43350.0920083796</v>
       </c>
     </row>
@@ -704,7 +709,7 @@
       <c r="A42" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="B42" s="0">
+      <c r="B42" s="1">
         <v>43350.0920083796</v>
       </c>
     </row>
@@ -712,7 +717,7 @@
       <c r="A43" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="B43" s="0">
+      <c r="B43" s="1">
         <v>43350.0920083796</v>
       </c>
     </row>
@@ -720,7 +725,7 @@
       <c r="A44" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="B44" s="0">
+      <c r="B44" s="1">
         <v>43350.0920083796</v>
       </c>
     </row>
@@ -728,7 +733,7 @@
       <c r="A45" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="B45" s="0">
+      <c r="B45" s="1">
         <v>43350.0920083796</v>
       </c>
     </row>
@@ -736,7 +741,7 @@
       <c r="A46" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="B46" s="0">
+      <c r="B46" s="1">
         <v>43350.0920083796</v>
       </c>
     </row>
@@ -744,7 +749,7 @@
       <c r="A47" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="B47" s="0">
+      <c r="B47" s="1">
         <v>43350.0920083796</v>
       </c>
     </row>
@@ -752,7 +757,7 @@
       <c r="A48" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="B48" s="0">
+      <c r="B48" s="1">
         <v>43350.0920083796</v>
       </c>
     </row>
@@ -760,7 +765,7 @@
       <c r="A49" s="0" t="s">
         <v>49</v>
       </c>
-      <c r="B49" s="0">
+      <c r="B49" s="1">
         <v>43350.0920083796</v>
       </c>
     </row>
@@ -768,7 +773,7 @@
       <c r="A50" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="B50" s="0">
+      <c r="B50" s="1">
         <v>43350.0920083796</v>
       </c>
     </row>
@@ -776,7 +781,7 @@
       <c r="A51" s="0" t="s">
         <v>51</v>
       </c>
-      <c r="B51" s="0">
+      <c r="B51" s="1">
         <v>43350.0920083796</v>
       </c>
     </row>
@@ -784,7 +789,7 @@
       <c r="A52" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="B52" s="0">
+      <c r="B52" s="1">
         <v>43350.0920083796</v>
       </c>
     </row>
@@ -792,7 +797,7 @@
       <c r="A53" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="B53" s="0">
+      <c r="B53" s="1">
         <v>43350.0920083796</v>
       </c>
     </row>
@@ -800,7 +805,7 @@
       <c r="A54" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="B54" s="0">
+      <c r="B54" s="1">
         <v>43350.0920083796</v>
       </c>
     </row>
@@ -808,7 +813,7 @@
       <c r="A55" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="B55" s="0">
+      <c r="B55" s="1">
         <v>43350.0920083796</v>
       </c>
     </row>
@@ -816,7 +821,7 @@
       <c r="A56" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="B56" s="0">
+      <c r="B56" s="1">
         <v>43350.0920083796</v>
       </c>
     </row>
@@ -824,7 +829,7 @@
       <c r="A57" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="B57" s="0">
+      <c r="B57" s="1">
         <v>43350.0920083796</v>
       </c>
     </row>
@@ -832,7 +837,7 @@
       <c r="A58" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="B58" s="0">
+      <c r="B58" s="1">
         <v>43350.0920083796</v>
       </c>
     </row>
@@ -840,7 +845,7 @@
       <c r="A59" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="B59" s="0">
+      <c r="B59" s="1">
         <v>43350.0920083796</v>
       </c>
     </row>
@@ -848,7 +853,7 @@
       <c r="A60" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="B60" s="0">
+      <c r="B60" s="1">
         <v>43350.0920083796</v>
       </c>
     </row>
@@ -856,7 +861,7 @@
       <c r="A61" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="B61" s="0">
+      <c r="B61" s="1">
         <v>43350.0920083796</v>
       </c>
     </row>
@@ -864,7 +869,7 @@
       <c r="A62" s="0" t="s">
         <v>62</v>
       </c>
-      <c r="B62" s="0">
+      <c r="B62" s="1">
         <v>43350.0920083796</v>
       </c>
     </row>
@@ -872,7 +877,7 @@
       <c r="A63" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="B63" s="0">
+      <c r="B63" s="1">
         <v>43350.0920083796</v>
       </c>
     </row>
@@ -880,7 +885,7 @@
       <c r="A64" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="B64" s="0">
+      <c r="B64" s="1">
         <v>43350.0920083796</v>
       </c>
     </row>
@@ -888,7 +893,7 @@
       <c r="A65" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="B65" s="0">
+      <c r="B65" s="1">
         <v>43350.0920083796</v>
       </c>
     </row>
@@ -896,7 +901,7 @@
       <c r="A66" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="B66" s="0">
+      <c r="B66" s="1">
         <v>43350.0920083796</v>
       </c>
     </row>
@@ -904,7 +909,7 @@
       <c r="A67" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="B67" s="0">
+      <c r="B67" s="1">
         <v>43350.0920083796</v>
       </c>
     </row>
@@ -912,7 +917,7 @@
       <c r="A68" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="B68" s="0">
+      <c r="B68" s="1">
         <v>43350.0920083796</v>
       </c>
     </row>
@@ -920,7 +925,7 @@
       <c r="A69" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="B69" s="0">
+      <c r="B69" s="1">
         <v>43350.0920083796</v>
       </c>
     </row>
@@ -928,7 +933,7 @@
       <c r="A70" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="B70" s="0">
+      <c r="B70" s="1">
         <v>43350.0920083796</v>
       </c>
     </row>
@@ -936,7 +941,7 @@
       <c r="A71" s="0" t="s">
         <v>71</v>
       </c>
-      <c r="B71" s="0">
+      <c r="B71" s="1">
         <v>43350.0920083796</v>
       </c>
     </row>
@@ -944,7 +949,7 @@
       <c r="A72" s="0" t="s">
         <v>72</v>
       </c>
-      <c r="B72" s="0">
+      <c r="B72" s="1">
         <v>43350.0920083796</v>
       </c>
     </row>
@@ -952,7 +957,7 @@
       <c r="A73" s="0" t="s">
         <v>73</v>
       </c>
-      <c r="B73" s="0">
+      <c r="B73" s="1">
         <v>43350.0920083796</v>
       </c>
     </row>
@@ -960,7 +965,7 @@
       <c r="A74" s="0" t="s">
         <v>74</v>
       </c>
-      <c r="B74" s="0">
+      <c r="B74" s="1">
         <v>43350.0920083796</v>
       </c>
     </row>
@@ -968,7 +973,7 @@
       <c r="A75" s="0" t="s">
         <v>75</v>
       </c>
-      <c r="B75" s="0">
+      <c r="B75" s="1">
         <v>43350.0920083796</v>
       </c>
     </row>
@@ -976,7 +981,7 @@
       <c r="A76" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="B76" s="0">
+      <c r="B76" s="1">
         <v>43350.0920083796</v>
       </c>
     </row>
@@ -984,7 +989,7 @@
       <c r="A77" s="0" t="s">
         <v>77</v>
       </c>
-      <c r="B77" s="0">
+      <c r="B77" s="1">
         <v>43350.0920083796</v>
       </c>
     </row>
@@ -992,7 +997,7 @@
       <c r="A78" s="0" t="s">
         <v>78</v>
       </c>
-      <c r="B78" s="0">
+      <c r="B78" s="1">
         <v>43350.0920083796</v>
       </c>
     </row>
@@ -1000,7 +1005,7 @@
       <c r="A79" s="0" t="s">
         <v>79</v>
       </c>
-      <c r="B79" s="0">
+      <c r="B79" s="1">
         <v>43350.0920083796</v>
       </c>
     </row>
@@ -1008,7 +1013,7 @@
       <c r="A80" s="0" t="s">
         <v>80</v>
       </c>
-      <c r="B80" s="0">
+      <c r="B80" s="1">
         <v>43350.0920083796</v>
       </c>
     </row>
@@ -1016,7 +1021,7 @@
       <c r="A81" s="0" t="s">
         <v>81</v>
       </c>
-      <c r="B81" s="0">
+      <c r="B81" s="1">
         <v>43350.0920083796</v>
       </c>
     </row>
@@ -1024,7 +1029,7 @@
       <c r="A82" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="B82" s="0">
+      <c r="B82" s="1">
         <v>43350.0920083796</v>
       </c>
     </row>
@@ -1032,7 +1037,7 @@
       <c r="A83" s="0" t="s">
         <v>83</v>
       </c>
-      <c r="B83" s="0">
+      <c r="B83" s="1">
         <v>43350.0920083796</v>
       </c>
     </row>
@@ -1040,7 +1045,7 @@
       <c r="A84" s="0" t="s">
         <v>84</v>
       </c>
-      <c r="B84" s="0">
+      <c r="B84" s="1">
         <v>43350.0920083796</v>
       </c>
     </row>
@@ -1048,7 +1053,7 @@
       <c r="A85" s="0" t="s">
         <v>85</v>
       </c>
-      <c r="B85" s="0">
+      <c r="B85" s="1">
         <v>43350.0920083796</v>
       </c>
     </row>
@@ -1056,7 +1061,7 @@
       <c r="A86" s="0" t="s">
         <v>86</v>
       </c>
-      <c r="B86" s="0">
+      <c r="B86" s="1">
         <v>43350.0920083796</v>
       </c>
     </row>
@@ -1064,7 +1069,7 @@
       <c r="A87" s="0" t="s">
         <v>87</v>
       </c>
-      <c r="B87" s="0">
+      <c r="B87" s="1">
         <v>43350.0920083796</v>
       </c>
     </row>
@@ -1072,7 +1077,7 @@
       <c r="A88" s="0" t="s">
         <v>88</v>
       </c>
-      <c r="B88" s="0">
+      <c r="B88" s="1">
         <v>43350.0920083796</v>
       </c>
     </row>
@@ -1080,7 +1085,7 @@
       <c r="A89" s="0" t="s">
         <v>89</v>
       </c>
-      <c r="B89" s="0">
+      <c r="B89" s="1">
         <v>43350.0920083796</v>
       </c>
     </row>
@@ -1088,7 +1093,7 @@
       <c r="A90" s="0" t="s">
         <v>90</v>
       </c>
-      <c r="B90" s="0">
+      <c r="B90" s="1">
         <v>43350.0920083796</v>
       </c>
     </row>
@@ -1096,7 +1101,7 @@
       <c r="A91" s="0" t="s">
         <v>91</v>
       </c>
-      <c r="B91" s="0">
+      <c r="B91" s="1">
         <v>43350.0920083796</v>
       </c>
     </row>
@@ -1104,7 +1109,7 @@
       <c r="A92" s="0" t="s">
         <v>92</v>
       </c>
-      <c r="B92" s="0">
+      <c r="B92" s="1">
         <v>43350.0920083796</v>
       </c>
     </row>
@@ -1112,7 +1117,7 @@
       <c r="A93" s="0" t="s">
         <v>93</v>
       </c>
-      <c r="B93" s="0">
+      <c r="B93" s="1">
         <v>43350.0920083796</v>
       </c>
     </row>
@@ -1120,7 +1125,7 @@
       <c r="A94" s="0" t="s">
         <v>94</v>
       </c>
-      <c r="B94" s="0">
+      <c r="B94" s="1">
         <v>43350.0920083796</v>
       </c>
     </row>
@@ -1128,7 +1133,7 @@
       <c r="A95" s="0" t="s">
         <v>95</v>
       </c>
-      <c r="B95" s="0">
+      <c r="B95" s="1">
         <v>43350.0920083796</v>
       </c>
     </row>
@@ -1136,7 +1141,7 @@
       <c r="A96" s="0" t="s">
         <v>96</v>
       </c>
-      <c r="B96" s="0">
+      <c r="B96" s="1">
         <v>43350.0920083796</v>
       </c>
     </row>
@@ -1144,7 +1149,7 @@
       <c r="A97" s="0" t="s">
         <v>97</v>
       </c>
-      <c r="B97" s="0">
+      <c r="B97" s="1">
         <v>43350.0920083796</v>
       </c>
     </row>

</xml_diff>